<commit_message>
adjusting things to KBar
adjusting to KBar
changed the plot_CA_CR to plot_garnet_geotherm
Added some warnings in terms of missing composition to the garnet_class.py
Changed Sudholz2021 xls file to make .15 change in temp
</commit_message>
<xml_diff>
--- a/Benchmarking/garnet/PT_Sudholz.xlsx
+++ b/Benchmarking/garnet/PT_Sudholz.xlsx
@@ -528,10 +528,10 @@
   <dimension ref="A1:N118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -589,7 +589,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>999.584718735689</v>
+        <v>999.434718735689</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>925.969146118349</v>
@@ -629,7 +629,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1248.57152506871</v>
+        <v>1248.42152506871</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>1057.97094758787</v>
@@ -673,7 +673,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>995.482141422758</v>
+        <v>995.332141422757</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>947.68779175408</v>
@@ -717,7 +717,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1069.50884327748</v>
+        <v>1069.35884327748</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>984.678861990497</v>
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1406.46493542644</v>
+        <v>1406.31493542644</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>1261.42161286537</v>
@@ -799,7 +799,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1257.81079959572</v>
+        <v>1257.66079959572</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1182.99655821858</v>
@@ -841,7 +841,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1268.67932234993</v>
+        <v>1268.52932234993</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1166.08083805694</v>
@@ -883,7 +883,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1207.88598329619</v>
+        <v>1207.7359832962</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>1146.19207903912</v>
@@ -927,7 +927,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1126.98166027161</v>
+        <v>1126.83166027161</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1134.51800539089</v>
@@ -971,7 +971,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1318.83540312989</v>
+        <v>1318.68540312989</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1241.14976189738</v>
@@ -1015,7 +1015,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1337.36937842617</v>
+        <v>1337.21937842617</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>1151.77185716811</v>
@@ -1057,7 +1057,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1243.34815135579</v>
+        <v>1243.1981513558</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>1229.02689655716</v>
@@ -1099,7 +1099,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1231.91027017817</v>
+        <v>1231.76027017817</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>1217.7398319456</v>
@@ -1143,7 +1143,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>1226.93113223859</v>
+        <v>1226.78113223859</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>1183.86868574283</v>
@@ -1187,7 +1187,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1222.12182853259</v>
+        <v>1221.97182853258</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>1156.05907694227</v>
@@ -1231,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>1431.3635005196</v>
+        <v>1431.2135005196</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>1224.25948959003</v>
@@ -1275,7 +1275,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1364.22802654784</v>
+        <v>1364.07802654784</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>1277.02400473062</v>
@@ -1319,7 +1319,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>1347.15526195077</v>
+        <v>1347.00526195077</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>1208.69436518816</v>
@@ -1363,7 +1363,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>932.235442643719</v>
+        <v>932.08544264372</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>906.312603239375</v>
@@ -1407,7 +1407,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1025.28581547163</v>
+        <v>1025.13581547163</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>949.104556717275</v>
@@ -1451,7 +1451,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>1164.32067476113</v>
+        <v>1164.17067476113</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>1113.0920116217</v>
@@ -1495,7 +1495,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>932.43759160136</v>
+        <v>932.287591601361</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>875.88617711382</v>
@@ -1539,7 +1539,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>942.543034838869</v>
+        <v>942.39303483887</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>911.11835265531</v>
@@ -1583,7 +1583,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>1239.67171539768</v>
+        <v>1239.52171539768</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>1097.12797781747</v>
@@ -1627,7 +1627,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1053.1829039571</v>
+        <v>1053.0329039571</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>1030.94771193996</v>
@@ -1671,7 +1671,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>1235.22117614707</v>
+        <v>1235.07117614707</v>
       </c>
       <c r="C27" s="4" t="n">
         <v>1119.58481586885</v>
@@ -1715,7 +1715,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1297.71099149229</v>
+        <v>1297.56099149229</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>1104.84754365031</v>
@@ -1759,7 +1759,7 @@
         <v>41</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>1217.88153791733</v>
+        <v>1217.73153791733</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>1163.44517253588</v>
@@ -1803,7 +1803,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1077.43735850427</v>
+        <v>1077.28735850427</v>
       </c>
       <c r="C30" s="4" t="n">
         <v>1014.75028395462</v>
@@ -1847,7 +1847,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>1268.36091197954</v>
+        <v>1268.21091197954</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>1135.78483297333</v>
@@ -1891,7 +1891,7 @@
         <v>44</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1114.4653117524</v>
+        <v>1114.31531175239</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>1122.2566094999</v>
@@ -1935,7 +1935,7 @@
         <v>45</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1044.46734670145</v>
+        <v>1044.31734670145</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>1013.28683316059</v>
@@ -1979,7 +1979,7 @@
         <v>46</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1159.26051357018</v>
+        <v>1159.11051357018</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>1084.21263415204</v>
@@ -2023,7 +2023,7 @@
         <v>47</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>1303.06573437443</v>
+        <v>1302.91573437443</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>1131.00797115409</v>
@@ -2067,7 +2067,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1176.937020263</v>
+        <v>1176.787020263</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>1104.07736712717</v>
@@ -2111,7 +2111,7 @@
         <v>49</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1168.52097187788</v>
+        <v>1168.37097187788</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>1097.12797781747</v>
@@ -2155,7 +2155,7 @@
         <v>50</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>899.948274047628</v>
+        <v>899.798274047627</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>848.973419762888</v>
@@ -2199,7 +2199,7 @@
         <v>51</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1203.21712625003</v>
+        <v>1203.06712625003</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>1094.7191244487</v>
@@ -2243,7 +2243,7 @@
         <v>52</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1234.9853127774</v>
+        <v>1234.8353127774</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>1101.51895149418</v>
@@ -2287,7 +2287,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>1123.1051251621</v>
+        <v>1122.9551251621</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>1072.84779100277</v>
@@ -2331,7 +2331,7 @@
         <v>54</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>1265.79369943339</v>
+        <v>1265.64369943339</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>1140.88367563885</v>
@@ -2375,7 +2375,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>1160.2117571661</v>
+        <v>1160.0617571661</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>1046.61199580219</v>
@@ -2419,7 +2419,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>1107.2080966063</v>
+        <v>1107.0580966063</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>1049.36146297974</v>
@@ -2463,7 +2463,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1061.48442233344</v>
+        <v>1061.33442233344</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>1051.20648074766</v>
@@ -2507,7 +2507,7 @@
         <v>58</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>1325.74900201548</v>
+        <v>1325.59900201548</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>1193.2789254512</v>
@@ -2551,7 +2551,7 @@
         <v>59</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>1041.98080477438</v>
+        <v>1041.83080477438</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>1022.17219960356</v>
@@ -2595,7 +2595,7 @@
         <v>60</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>1039.16433387949</v>
+        <v>1039.01433387949</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>1016.79482006175</v>
@@ -2639,7 +2639,7 @@
         <v>61</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>1267.04349551031</v>
+        <v>1266.89349551032</v>
       </c>
       <c r="C49" s="4" t="n">
         <v>1119.5209327789</v>
@@ -2683,7 +2683,7 @@
         <v>62</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>1207.46269132528</v>
+        <v>1207.31269132528</v>
       </c>
       <c r="C50" s="4" t="n">
         <v>1148.84368153664</v>
@@ -2727,7 +2727,7 @@
         <v>63</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1152.63580007646</v>
+        <v>1152.48580007646</v>
       </c>
       <c r="C51" s="4" t="n">
         <v>1136.63500216256</v>
@@ -2771,7 +2771,7 @@
         <v>64</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>1139.57203004584</v>
+        <v>1139.42203004584</v>
       </c>
       <c r="C52" s="4" t="n">
         <v>1147.08433627995</v>
@@ -2815,7 +2815,7 @@
         <v>65</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>1125.11423642407</v>
+        <v>1124.96423642407</v>
       </c>
       <c r="C53" s="4" t="n">
         <v>1135.41981005869</v>
@@ -2859,7 +2859,7 @@
         <v>66</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>1129.18708399983</v>
+        <v>1129.03708399984</v>
       </c>
       <c r="C54" s="4" t="n">
         <v>1145.31583895709</v>
@@ -2903,7 +2903,7 @@
         <v>67</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>1108.59280802607</v>
+        <v>1108.44280802607</v>
       </c>
       <c r="C55" s="4" t="n">
         <v>1126.78646312871</v>
@@ -2947,7 +2947,7 @@
         <v>68</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>1141.44574695669</v>
+        <v>1141.29574695669</v>
       </c>
       <c r="C56" s="4" t="n">
         <v>1159.21420987061</v>
@@ -2991,7 +2991,7 @@
         <v>69</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>1072.58502372615</v>
+        <v>1072.43502372615</v>
       </c>
       <c r="C57" s="4" t="n">
         <v>1026.13638030443</v>
@@ -3035,7 +3035,7 @@
         <v>70</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>1041.32061222701</v>
+        <v>1041.17061222701</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>1008.05370240209</v>
@@ -3079,7 +3079,7 @@
         <v>71</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>1083.34840154806</v>
+        <v>1083.19840154806</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>1003.33460047701</v>
@@ -3123,7 +3123,7 @@
         <v>72</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>1212.83536233955</v>
+        <v>1212.68536233955</v>
       </c>
       <c r="C60" s="4" t="n">
         <v>1152.3354007409</v>
@@ -3167,7 +3167,7 @@
         <v>73</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>1293.98698086486</v>
+        <v>1293.83698086486</v>
       </c>
       <c r="C61" s="4" t="n">
         <v>1203.45754176162</v>
@@ -3211,7 +3211,7 @@
         <v>74</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>1029.31811670675</v>
+        <v>1029.16811670675</v>
       </c>
       <c r="C62" s="4" t="n">
         <v>988.641158584623</v>
@@ -3255,7 +3255,7 @@
         <v>75</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>972.093857888901</v>
+        <v>971.943857888901</v>
       </c>
       <c r="C63" s="4" t="n">
         <v>962.078882214477</v>
@@ -3299,7 +3299,7 @@
         <v>76</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>1019.29475996639</v>
+        <v>1019.14475996639</v>
       </c>
       <c r="C64" s="4" t="n">
         <v>998.52890942806</v>
@@ -3343,7 +3343,7 @@
         <v>77</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>1196.67488313575</v>
+        <v>1196.52488313575</v>
       </c>
       <c r="C65" s="4" t="n">
         <v>1163.72542120457</v>
@@ -3387,7 +3387,7 @@
         <v>78</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>1050.30131811901</v>
+        <v>1050.15131811901</v>
       </c>
       <c r="C66" s="4" t="n">
         <v>1008.05370240209</v>
@@ -3431,7 +3431,7 @@
         <v>79</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>936.888087904105</v>
+        <v>936.738087904105</v>
       </c>
       <c r="C67" s="4" t="n">
         <v>912.26551977275</v>
@@ -3475,7 +3475,7 @@
         <v>80</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>917.27488689946</v>
+        <v>917.124886899459</v>
       </c>
       <c r="C68" s="4" t="n">
         <v>932.231292471864</v>
@@ -3519,7 +3519,7 @@
         <v>81</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>1389.80287403117</v>
+        <v>1389.65287403117</v>
       </c>
       <c r="C69" s="4" t="n">
         <v>1290.88338403662</v>
@@ -3563,7 +3563,7 @@
         <v>82</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>1021.12177669783</v>
+        <v>1020.97177669783</v>
       </c>
       <c r="C70" s="4" t="n">
         <v>1026.57330961424</v>
@@ -3605,7 +3605,7 @@
         <v>83</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>1181.71538401383</v>
+        <v>1181.56538401383</v>
       </c>
       <c r="C71" s="4" t="n">
         <v>1099.41626095537</v>
@@ -3649,7 +3649,7 @@
         <v>84</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>1284.97976212778</v>
+        <v>1284.82976212778</v>
       </c>
       <c r="C72" s="4" t="n">
         <v>1250.64566907871</v>
@@ -3693,7 +3693,7 @@
         <v>85</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>985.746504123325</v>
+        <v>985.596504123325</v>
       </c>
       <c r="C73" s="4" t="n">
         <v>1001.42293625985</v>
@@ -3737,7 +3737,7 @@
         <v>86</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>1178.09716514553</v>
+        <v>1177.94716514553</v>
       </c>
       <c r="C74" s="4" t="n">
         <v>1089.31752463217</v>
@@ -3781,7 +3781,7 @@
         <v>86</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>1170.63637622484</v>
+        <v>1170.48637622484</v>
       </c>
       <c r="C75" s="4" t="n">
         <v>1082.02408142177</v>
@@ -3825,7 +3825,7 @@
         <v>87</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>1171.20390553368</v>
+        <v>1171.05390553368</v>
       </c>
       <c r="C76" s="4" t="n">
         <v>1136.42266289993</v>
@@ -3869,7 +3869,7 @@
         <v>87</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>1183.96160034368</v>
+        <v>1183.81160034368</v>
       </c>
       <c r="C77" s="4" t="n">
         <v>1146.05383299514</v>
@@ -3913,7 +3913,7 @@
         <v>88</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>1143.58559630082</v>
+        <v>1143.43559630082</v>
       </c>
       <c r="C78" s="4" t="n">
         <v>1112.8070564452</v>
@@ -3957,7 +3957,7 @@
         <v>88</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>1127.25774966873</v>
+        <v>1127.10774966873</v>
       </c>
       <c r="C79" s="4" t="n">
         <v>1095.96029673487</v>
@@ -4001,7 +4001,7 @@
         <v>89</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>1193.25999597429</v>
+        <v>1193.10999597429</v>
       </c>
       <c r="C80" s="4" t="n">
         <v>1127.44186021587</v>
@@ -4045,7 +4045,7 @@
         <v>89</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>1162.25367893527</v>
+        <v>1162.10367893527</v>
       </c>
       <c r="C81" s="4" t="n">
         <v>1105.51573767974</v>
@@ -4089,7 +4089,7 @@
         <v>90</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1064.75304539785</v>
+        <v>1064.60304539785</v>
       </c>
       <c r="C82" s="4" t="n">
         <v>1056.04308631902</v>
@@ -4133,7 +4133,7 @@
         <v>90</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>1061.12720275449</v>
+        <v>1060.97720275449</v>
       </c>
       <c r="C83" s="4" t="n">
         <v>1053.99151661683</v>
@@ -4177,7 +4177,7 @@
         <v>91</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>967.008955392465</v>
+        <v>966.858955392465</v>
       </c>
       <c r="C84" s="4" t="n">
         <v>965.033875089738</v>
@@ -4221,7 +4221,7 @@
         <v>91</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>993.972604989183</v>
+        <v>993.822604989183</v>
       </c>
       <c r="C85" s="4" t="n">
         <v>986.057441173184</v>
@@ -4265,7 +4265,7 @@
         <v>92</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>1248.46424040766</v>
+        <v>1248.31424040766</v>
       </c>
       <c r="C86" s="4" t="n">
         <v>1101.34990190892</v>
@@ -4309,7 +4309,7 @@
         <v>92</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>1243.57369973014</v>
+        <v>1243.42369973014</v>
       </c>
       <c r="C87" s="4" t="n">
         <v>1095.47820845433</v>
@@ -4353,7 +4353,7 @@
         <v>93</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>1087.24232699575</v>
+        <v>1087.09232699575</v>
       </c>
       <c r="C88" s="4" t="n">
         <v>1099.07578979291</v>
@@ -4397,7 +4397,7 @@
         <v>94</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>1101.59497494762</v>
+        <v>1101.44497494762</v>
       </c>
       <c r="C89" s="4" t="n">
         <v>1109.13280496708</v>
@@ -4441,7 +4441,7 @@
         <v>95</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>1322.65222251949</v>
+        <v>1322.50222251949</v>
       </c>
       <c r="C90" s="4" t="n">
         <v>1148.9752669025</v>
@@ -4485,7 +4485,7 @@
         <v>96</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>1320.77933137783</v>
+        <v>1320.62933137783</v>
       </c>
       <c r="C91" s="4" t="n">
         <v>1082.01327892661</v>
@@ -4529,7 +4529,7 @@
         <v>97</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>1199.42027945373</v>
+        <v>1199.27027945373</v>
       </c>
       <c r="C92" s="4" t="n">
         <v>1141.89421084105</v>
@@ -4573,7 +4573,7 @@
         <v>98</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>1413.76917920201</v>
+        <v>1413.61917920201</v>
       </c>
       <c r="C93" s="4" t="n">
         <v>1202.18522148265</v>
@@ -4617,7 +4617,7 @@
         <v>99</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>1192.43024466229</v>
+        <v>1192.28024466229</v>
       </c>
       <c r="C94" s="4" t="n">
         <v>1038.62622454043</v>
@@ -4661,7 +4661,7 @@
         <v>100</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>1122.26692505525</v>
+        <v>1122.11692505525</v>
       </c>
       <c r="C95" s="4" t="n">
         <v>1088.54662899357</v>
@@ -4705,7 +4705,7 @@
         <v>101</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>1188.42127551861</v>
+        <v>1188.27127551861</v>
       </c>
       <c r="C96" s="4" t="n">
         <v>1151.02727237459</v>
@@ -4749,7 +4749,7 @@
         <v>102</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>1112.87979473111</v>
+        <v>1112.72979473111</v>
       </c>
       <c r="C97" s="4" t="n">
         <v>1103.46658631133</v>
@@ -4793,7 +4793,7 @@
         <v>103</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>1225.70236257775</v>
+        <v>1225.55236257775</v>
       </c>
       <c r="C98" s="4" t="n">
         <v>1133.48153714733</v>
@@ -4837,7 +4837,7 @@
         <v>104</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>1173.71003999179</v>
+        <v>1173.56003999179</v>
       </c>
       <c r="C99" s="4" t="n">
         <v>1133.75388260058</v>
@@ -4881,7 +4881,7 @@
         <v>105</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>932.842379889659</v>
+        <v>932.692379889659</v>
       </c>
       <c r="C100" s="4" t="n">
         <v>934.134041892545</v>
@@ -4925,7 +4925,7 @@
         <v>106</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>944.032252576963</v>
+        <v>943.882252576963</v>
       </c>
       <c r="C101" s="4" t="n">
         <v>912.26551977275</v>
@@ -4969,7 +4969,7 @@
         <v>107</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>940.136950164923</v>
+        <v>939.986950164923</v>
       </c>
       <c r="C102" s="4" t="n">
         <v>923.796918918816</v>
@@ -5013,7 +5013,7 @@
         <v>108</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>883.917928697609</v>
+        <v>883.76792869761</v>
       </c>
       <c r="C103" s="4" t="n">
         <v>905.188979707737</v>
@@ -5057,7 +5057,7 @@
         <v>109</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>1080.56192737017</v>
+        <v>1080.41192737017</v>
       </c>
       <c r="C104" s="4" t="n">
         <v>1074.25520039066</v>
@@ -5101,7 +5101,7 @@
         <v>110</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>1080.34824457287</v>
+        <v>1080.19824457287</v>
       </c>
       <c r="C105" s="4" t="n">
         <v>1026.13638030443</v>
@@ -5145,7 +5145,7 @@
         <v>111</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>893.562527037415</v>
+        <v>893.412527037415</v>
       </c>
       <c r="C106" s="4" t="n">
         <v>925.77142446422</v>
@@ -5189,7 +5189,7 @@
         <v>112</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>1119.77888790491</v>
+        <v>1119.62888790491</v>
       </c>
       <c r="C107" s="4" t="n">
         <v>1072.40196175367</v>
@@ -5233,7 +5233,7 @@
         <v>113</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>1080.21300441917</v>
+        <v>1080.06300441917</v>
       </c>
       <c r="C108" s="4" t="n">
         <v>1042.27219544276</v>
@@ -5277,7 +5277,7 @@
         <v>114</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>1101.43075118736</v>
+        <v>1101.28075118736</v>
       </c>
       <c r="C109" s="4" t="n">
         <v>1055.57094055685</v>
@@ -5321,7 +5321,7 @@
         <v>115</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>951.669289917139</v>
+        <v>951.519289917139</v>
       </c>
       <c r="C110" s="4" t="n">
         <v>948.223417946709</v>
@@ -5365,7 +5365,7 @@
         <v>116</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>1090.64838120677</v>
+        <v>1090.49838120677</v>
       </c>
       <c r="C111" s="4" t="n">
         <v>1023.05813161966</v>
@@ -5409,7 +5409,7 @@
         <v>117</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>1023.03779369413</v>
+        <v>1022.88779369413</v>
       </c>
       <c r="C112" s="4" t="n">
         <v>1021.28336575814</v>
@@ -5453,7 +5453,7 @@
         <v>118</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>1042.69318703156</v>
+        <v>1042.54318703156</v>
       </c>
       <c r="C113" s="4" t="n">
         <v>1032.19099076156</v>
@@ -5497,7 +5497,7 @@
         <v>119</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>1346.26953684146</v>
+        <v>1346.11953684146</v>
       </c>
       <c r="C114" s="4" t="n">
         <v>1234.76864481242</v>
@@ -5541,7 +5541,7 @@
         <v>120</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>1367.61187621501</v>
+        <v>1367.461876215</v>
       </c>
       <c r="C115" s="4" t="n">
         <v>1237.07584448953</v>
@@ -5585,7 +5585,7 @@
         <v>121</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>1296.71339350935</v>
+        <v>1296.56339350935</v>
       </c>
       <c r="C116" s="4" t="n">
         <v>1215.80426612755</v>
@@ -5629,7 +5629,7 @@
         <v>122</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>1346.38333063423</v>
+        <v>1346.23333063423</v>
       </c>
       <c r="C117" s="4" t="n">
         <v>1227.76483435625</v>
@@ -5673,7 +5673,7 @@
         <v>123</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>1128.54265575356</v>
+        <v>1128.39265575356</v>
       </c>
       <c r="C118" s="4" t="n">
         <v>1134.50549832382</v>

</xml_diff>